<commit_message>
Added some more graphs. Lines removed against commits
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -8,13 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Lenovo\Documents\code\SCons-Make-Research\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1560AE23-8BBD-4760-A2B7-7FAEEC1A0101}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2722AE9-05C3-41D0-BD91-FF1EC0438595}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SConstruct" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">SConstruct!$O$2</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">SConstruct!$O$3:$O$98</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">SConstruct!$P$2</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">SConstruct!$P$3:$P$98</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">SConstruct!$O$2</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">SConstruct!$O$3:$O$98</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">SConstruct!$P$2</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">SConstruct!$P$3:$P$98</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -28,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Repository age (EPOCH)</t>
   </si>
@@ -97,6 +107,12 @@
   </si>
   <si>
     <t>EPOCHS (Start of year)</t>
+  </si>
+  <si>
+    <t>Make total lines removed</t>
+  </si>
+  <si>
+    <t>Scons total lines removed</t>
   </si>
 </sst>
 </file>
@@ -1418,6 +1434,1724 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>No. Lines removed against No. Commits (Make)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>What (Make)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SConstruct!$I$3:$I$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="71"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SConstruct!$N$3:$N$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="71"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B94B-48A5-8A3D-949FF5DADCBB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="713838064"/>
+        <c:axId val="1031981328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="713838064"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>No.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> Commits</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1031981328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1031981328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>No. lines removed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="713838064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>No. Lines removed against No. Commits (Scons)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SConstruct!$B$3:$B$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="71"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SConstruct!$O$3:$O$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="71"/>
+                <c:pt idx="0">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6696</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:v>What (Make)</c:v>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B611-4360-92EA-233801CD4020}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="713838064"/>
+        <c:axId val="1031981328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="713838064"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>No.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> Commits</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1031981328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1031981328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>No. lines removed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="713838064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1498,6 +3232,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2485,6 +4299,1038 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2573,6 +5419,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>99218</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>84931</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>916781</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>89694</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{633F29B4-D8BC-4A6C-8CE0-EA2BADE99689}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>87313</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>63499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>904876</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B04130C9-07EA-4154-8FF7-529DF0ED9711}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2878,10 +5798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2898,6 +5818,9 @@
     <col min="10" max="10" width="16.26953125" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="12" width="17.90625" customWidth="1"/>
+    <col min="14" max="14" width="22.26953125" customWidth="1"/>
+    <col min="15" max="15" width="22.6328125" customWidth="1"/>
+    <col min="16" max="16" width="16" customWidth="1"/>
     <col min="19" max="19" width="20.26953125" customWidth="1"/>
     <col min="20" max="20" width="17" customWidth="1"/>
     <col min="21" max="21" width="20.26953125" customWidth="1"/>
@@ -2907,7 +5830,7 @@
     <col min="26" max="26" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2921,7 +5844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2950,8 +5873,14 @@
       <c r="L2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1011660709</v>
       </c>
@@ -2984,8 +5913,14 @@
       <c r="L3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1011660709</v>
       </c>
@@ -3019,8 +5954,14 @@
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1034422658</v>
       </c>
@@ -3050,8 +5991,14 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1043968983</v>
       </c>
@@ -3085,8 +6032,14 @@
         <f>I3</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1105019550</v>
       </c>
@@ -3119,8 +6072,14 @@
       <c r="L7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1176413691</v>
       </c>
@@ -3152,8 +6111,14 @@
         <f>AVERAGE(I4:I5)</f>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <v>194</v>
+      </c>
+      <c r="O8">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1207339321</v>
       </c>
@@ -3187,8 +6152,14 @@
         <f>AVERAGE(I6:I9)</f>
         <v>8.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1237799935</v>
       </c>
@@ -3225,8 +6196,14 @@
         <f>AVERAGE(I10:I13)</f>
         <v>11.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1237860221</v>
       </c>
@@ -3258,8 +6235,14 @@
         <f>AVERAGE(I14:I16)</f>
         <v>4.333333333333333</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N11">
+        <v>39</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1253670590</v>
       </c>
@@ -3291,8 +6274,14 @@
         <f>AVERAGE(I17:I24)</f>
         <v>8.25</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1256766229</v>
       </c>
@@ -3324,8 +6313,14 @@
         <f>AVERAGE(I25:I43)</f>
         <v>10.473684210526315</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N13">
+        <v>318</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1266842558</v>
       </c>
@@ -3362,8 +6357,14 @@
         <f>AVERAGE(I44:I60)</f>
         <v>4.882352941176471</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1283229025</v>
       </c>
@@ -3395,8 +6396,14 @@
         <f>AVERAGE(I61:I67)</f>
         <v>3.4285714285714284</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1297682135</v>
       </c>
@@ -3430,8 +6437,14 @@
         <f>AVERAGE(I68:I72)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N16">
+        <v>194</v>
+      </c>
+      <c r="O16">
+        <v>6696</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1298894081</v>
       </c>
@@ -3466,8 +6479,14 @@
         <f>AVERAGE(I73)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N17">
+        <v>176</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1299789239</v>
       </c>
@@ -3498,8 +6517,14 @@
       <c r="L18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N18">
+        <v>19</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1306259723</v>
       </c>
@@ -3513,8 +6538,14 @@
       <c r="I19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N19">
+        <v>4</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1314799558</v>
       </c>
@@ -3528,8 +6559,14 @@
       <c r="I20">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N20">
+        <v>5</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1315200408</v>
       </c>
@@ -3543,8 +6580,14 @@
       <c r="I21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N21">
+        <v>18</v>
+      </c>
+      <c r="O21">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1315445249</v>
       </c>
@@ -3558,8 +6601,14 @@
       <c r="I22">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1320407798</v>
       </c>
@@ -3573,8 +6622,14 @@
       <c r="I23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N23">
+        <v>4</v>
+      </c>
+      <c r="O23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1322330353</v>
       </c>
@@ -3588,8 +6643,14 @@
       <c r="I24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N24">
+        <v>26</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1332474676</v>
       </c>
@@ -3608,8 +6669,14 @@
       <c r="J25" s="1">
         <v>2014</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N25">
+        <v>5</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1332980051</v>
       </c>
@@ -3623,8 +6690,14 @@
       <c r="I26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N26">
+        <v>230</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1333947798</v>
       </c>
@@ -3638,8 +6711,14 @@
       <c r="I27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1342094874</v>
       </c>
@@ -3653,8 +6732,14 @@
       <c r="I28">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1342637455</v>
       </c>
@@ -3668,8 +6753,14 @@
       <c r="I29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1346341630</v>
       </c>
@@ -3683,8 +6774,14 @@
       <c r="I30">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N30">
+        <v>8</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1348000436</v>
       </c>
@@ -3698,8 +6795,14 @@
       <c r="I31">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N31">
+        <v>47</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1351114087</v>
       </c>
@@ -3713,8 +6816,14 @@
       <c r="I32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N32">
+        <v>37</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1354381046</v>
       </c>
@@ -3728,8 +6837,14 @@
       <c r="I33">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N33">
+        <v>22</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1357278519</v>
       </c>
@@ -3745,8 +6860,14 @@
       <c r="I34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1360718707</v>
       </c>
@@ -3760,8 +6881,14 @@
       <c r="I35">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N35">
+        <v>19</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1370204000</v>
       </c>
@@ -3775,8 +6902,14 @@
       <c r="I36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N36">
+        <v>5</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1370826833</v>
       </c>
@@ -3790,8 +6923,14 @@
       <c r="I37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1381535033</v>
       </c>
@@ -3805,8 +6944,14 @@
       <c r="I38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N38">
+        <v>42</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1389397070</v>
       </c>
@@ -3822,8 +6967,14 @@
       <c r="I39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N39">
+        <v>10</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1390609370</v>
       </c>
@@ -3837,8 +6988,14 @@
       <c r="I40">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1392085662</v>
       </c>
@@ -3852,8 +7009,14 @@
       <c r="I41">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N41">
+        <v>17</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1394046157</v>
       </c>
@@ -3867,8 +7030,14 @@
       <c r="I42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N42">
+        <v>55</v>
+      </c>
+      <c r="O42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1402921179</v>
       </c>
@@ -3882,8 +7051,14 @@
       <c r="I43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N43">
+        <v>2</v>
+      </c>
+      <c r="O43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1406140457</v>
       </c>
@@ -3900,8 +7075,14 @@
       <c r="J44" s="1">
         <v>2015</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1408490281</v>
       </c>
@@ -3915,8 +7096,14 @@
       <c r="I45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1409153544</v>
       </c>
@@ -3930,8 +7117,14 @@
       <c r="I46">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1409750299</v>
       </c>
@@ -3945,8 +7138,14 @@
       <c r="I47">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1413278657</v>
       </c>
@@ -3960,8 +7159,14 @@
       <c r="I48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N48">
+        <v>17</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1417504653</v>
       </c>
@@ -3975,8 +7180,14 @@
       <c r="I49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N49">
+        <v>4</v>
+      </c>
+      <c r="O49">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1417801488</v>
       </c>
@@ -3990,8 +7201,14 @@
       <c r="I50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1428876281</v>
       </c>
@@ -4007,8 +7224,14 @@
       <c r="I51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N51">
+        <v>43</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1430510164</v>
       </c>
@@ -4022,8 +7245,14 @@
       <c r="I52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1430925380</v>
       </c>
@@ -4037,8 +7266,14 @@
       <c r="I53">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N53">
+        <v>51</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1434653100</v>
       </c>
@@ -4052,8 +7287,14 @@
       <c r="I54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N54">
+        <v>9</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1442661280</v>
       </c>
@@ -4067,8 +7308,14 @@
       <c r="I55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N55">
+        <v>87</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1449368275</v>
       </c>
@@ -4084,8 +7331,14 @@
       </c>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N56">
+        <v>3</v>
+      </c>
+      <c r="O56">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1452698004</v>
       </c>
@@ -4103,8 +7356,14 @@
       </c>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N57">
+        <v>28</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1453435001</v>
       </c>
@@ -4120,8 +7379,14 @@
       </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1454464594</v>
       </c>
@@ -4137,8 +7402,14 @@
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1454782656</v>
       </c>
@@ -4152,8 +7423,14 @@
       <c r="I60">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1457612258</v>
       </c>
@@ -4170,8 +7447,14 @@
       <c r="J61" s="1">
         <v>2016</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1461716054</v>
       </c>
@@ -4185,8 +7468,14 @@
       <c r="I62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1465194671</v>
       </c>
@@ -4200,8 +7489,14 @@
       <c r="I63">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N63">
+        <v>16</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1466016288</v>
       </c>
@@ -4215,8 +7510,14 @@
       <c r="I64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N64">
+        <v>17</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1467255205</v>
       </c>
@@ -4230,8 +7531,14 @@
       <c r="I65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1477854720</v>
       </c>
@@ -4245,8 +7552,14 @@
       <c r="I66">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1488826636</v>
       </c>
@@ -4262,8 +7575,14 @@
       <c r="I67">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N67">
+        <v>27</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1490184268</v>
       </c>
@@ -4280,8 +7599,14 @@
       <c r="J68" s="1">
         <v>2017</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N68">
+        <v>1</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1496071665</v>
       </c>
@@ -4295,8 +7620,14 @@
       <c r="I69">
         <v>17</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N69">
+        <v>3</v>
+      </c>
+      <c r="O69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1496349016</v>
       </c>
@@ -4310,8 +7641,14 @@
       <c r="I70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N70">
+        <v>3</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1498090728</v>
       </c>
@@ -4325,8 +7662,14 @@
       <c r="I71">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N71">
+        <v>492</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1499234528</v>
       </c>
@@ -4340,8 +7683,14 @@
       <c r="I72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N72">
+        <v>58</v>
+      </c>
+      <c r="O72">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1500339182</v>
       </c>
@@ -4358,8 +7707,14 @@
       <c r="J73" s="1">
         <v>2018</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N73">
+        <v>9</v>
+      </c>
+      <c r="O73">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1500537826</v>
       </c>
@@ -4367,8 +7722,11 @@
         <v>20</v>
       </c>
       <c r="C74" s="1"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="O74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1502494929</v>
       </c>
@@ -4376,8 +7734,11 @@
         <v>1</v>
       </c>
       <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="O75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1504609799</v>
       </c>
@@ -4385,8 +7746,11 @@
         <v>1</v>
       </c>
       <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="O76">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1509043599</v>
       </c>
@@ -4394,8 +7758,11 @@
         <v>1</v>
       </c>
       <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="O77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1509980917</v>
       </c>
@@ -4403,8 +7770,11 @@
         <v>1</v>
       </c>
       <c r="C78" s="1"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="O78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1510627730</v>
       </c>
@@ -4412,8 +7782,11 @@
         <v>1</v>
       </c>
       <c r="C79" s="1"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="O79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1513433461</v>
       </c>
@@ -4421,8 +7794,11 @@
         <v>1</v>
       </c>
       <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O80">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1513502366</v>
       </c>
@@ -4430,8 +7806,11 @@
         <v>2</v>
       </c>
       <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1514105016</v>
       </c>
@@ -4439,8 +7818,11 @@
         <v>1</v>
       </c>
       <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1515425925</v>
       </c>
@@ -4450,8 +7832,11 @@
       <c r="C83" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1520258352</v>
       </c>
@@ -4459,8 +7844,11 @@
         <v>1</v>
       </c>
       <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1520325457</v>
       </c>
@@ -4468,8 +7856,11 @@
         <v>1</v>
       </c>
       <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>1521427474</v>
       </c>
@@ -4477,8 +7868,11 @@
         <v>4</v>
       </c>
       <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>1524250714</v>
       </c>
@@ -4486,8 +7880,11 @@
         <v>1</v>
       </c>
       <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1532509459</v>
       </c>
@@ -4495,8 +7892,11 @@
         <v>1</v>
       </c>
       <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O88">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1533588545</v>
       </c>
@@ -4504,8 +7904,11 @@
         <v>2</v>
       </c>
       <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O89">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1540966450</v>
       </c>
@@ -4513,8 +7916,11 @@
         <v>2</v>
       </c>
       <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1541901013</v>
       </c>
@@ -4522,8 +7928,11 @@
         <v>1</v>
       </c>
       <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O91">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1542819512</v>
       </c>
@@ -4531,8 +7940,11 @@
         <v>1</v>
       </c>
       <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1543443398</v>
       </c>
@@ -4540,8 +7952,11 @@
         <v>1</v>
       </c>
       <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1544565019</v>
       </c>
@@ -4549,8 +7964,11 @@
         <v>1</v>
       </c>
       <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O94">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1548861450</v>
       </c>
@@ -4560,8 +7978,11 @@
       <c r="C95" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O95">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>1552745223</v>
       </c>
@@ -4569,8 +7990,11 @@
         <v>1</v>
       </c>
       <c r="C96" s="1"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>1555035076</v>
       </c>
@@ -4578,8 +8002,11 @@
         <v>3</v>
       </c>
       <c r="C97" s="1"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="O97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>1558985607</v>
       </c>
@@ -4587,6 +8014,9 @@
         <v>1</v>
       </c>
       <c r="C98" s="1"/>
+      <c r="O98">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:D17">

</xml_diff>

<commit_message>
Fixed a mistake where the graph was using an incorrectly sorted commit list which threw the results off
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -8,23 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Lenovo\Documents\code\SCons-Make-Research\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2722AE9-05C3-41D0-BD91-FF1EC0438595}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CEE990-1348-4502-9BD8-7BECDFEE0EEF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SConstruct" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">SConstruct!$O$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">SConstruct!$O$3:$O$98</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">SConstruct!$P$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">SConstruct!$P$3:$P$98</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">SConstruct!$O$2</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">SConstruct!$O$3:$O$98</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">SConstruct!$P$2</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">SConstruct!$P$3:$P$98</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Repository age (EPOCH)</t>
   </si>
@@ -109,10 +99,10 @@
     <t>EPOCHS (Start of year)</t>
   </si>
   <si>
-    <t>Make total lines removed</t>
+    <t>Total lines removed</t>
   </si>
   <si>
-    <t>Scons total lines removed</t>
+    <t>Total commits (Unsorted)</t>
   </si>
 </sst>
 </file>
@@ -693,8 +683,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Average no. commits per year (SCons)</a:t>
+              <a:rPr lang="en-US" sz="1000"/>
+              <a:t>Average no. commits per year</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -739,15 +729,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>SConstruct!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ave commits per year</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>SCons</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -875,6 +857,85 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0FD7-4949-A244-E6FFC9137432}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Make</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>SConstruct!$L$3:$L$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.473684210526315</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.882352941176471</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.4285714285714284</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-05EB-4F1B-9737-E55F9B374524}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1007,6 +1068,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1024,7 +1116,14 @@
       </a:solidFill>
       <a:round/>
     </a:ln>
-    <a:effectLst/>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+        <a:srgbClr val="000000">
+          <a:alpha val="10000"/>
+        </a:srgbClr>
+      </a:outerShdw>
+      <a:softEdge rad="12700"/>
+    </a:effectLst>
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
@@ -1078,397 +1177,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-AU"/>
-              <a:t>Ave commits no.</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> commits per yeat (Make)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>SConstruct!$L$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ave commits per year</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>SConstruct!$K$3:$K$18</c:f>
-              <c:strCache>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>Pre-2005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2019</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>SConstruct!$L$3:$L$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.333333333333333</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10.473684210526315</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.882352941176471</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.4285714285714284</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1F87-4F7B-B044-96A323AA39EE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1445568176"/>
-        <c:axId val="1237008368"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1445568176"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1237008368"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1237008368"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1445568176"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="900"/>
               <a:t>No. Lines removed against No. Commits (Make)</a:t>
             </a:r>
           </a:p>
@@ -1539,222 +1248,222 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SConstruct!$I$3:$I$73</c:f>
+              <c:f>SConstruct!$O$3:$O$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>85</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>31</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="30">
-                  <c:v>24</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="39">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="44">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="46">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="47">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="52">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="55">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="53">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>8</c:v>
-                </c:pt>
                 <c:pt idx="56">
-                  <c:v>20</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="60">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="67">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="64">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="68">
-                  <c:v>9</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2041,14 +1750,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-AU"/>
+                  <a:rPr lang="en-AU" sz="700"/>
                   <a:t>No.</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:rPr lang="en-AU" sz="700" baseline="0"/>
                   <a:t> Commits</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-AU"/>
+                <a:endParaRPr lang="en-AU" sz="700"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2163,7 +1872,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-AU"/>
+                  <a:rPr lang="en-AU" sz="700"/>
                   <a:t>No. lines removed</a:t>
                 </a:r>
               </a:p>
@@ -2271,7 +1980,14 @@
       </a:solidFill>
       <a:round/>
     </a:ln>
-    <a:effectLst/>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+        <a:srgbClr val="000000">
+          <a:alpha val="10000"/>
+        </a:srgbClr>
+      </a:outerShdw>
+      <a:softEdge rad="12700"/>
+    </a:effectLst>
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
@@ -2291,7 +2007,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2325,7 +2041,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="900"/>
               <a:t>No. Lines removed against No. Commits (Scons)</a:t>
             </a:r>
           </a:p>
@@ -2393,198 +2109,198 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SConstruct!$B$3:$B$73</c:f>
+              <c:f>SConstruct!$Q$3:$Q$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>337</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>44</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>56</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="28">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="31">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>10</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="44">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="42">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="46">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="48">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="52">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="56">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="57">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>2</c:v>
@@ -2596,7 +2312,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>1</c:v>
@@ -2605,17 +2321,17 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>3</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SConstruct!$O$3:$O$73</c:f>
+              <c:f>SConstruct!$P$3:$P$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
@@ -2902,14 +2618,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-AU"/>
+                  <a:rPr lang="en-AU" sz="700"/>
                   <a:t>No.</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:rPr lang="en-AU" sz="700" baseline="0"/>
                   <a:t> Commits</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-AU"/>
+                <a:endParaRPr lang="en-AU" sz="700"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3024,7 +2740,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-AU"/>
+                  <a:rPr lang="en-AU" sz="700"/>
                   <a:t>No. lines removed</a:t>
                 </a:r>
               </a:p>
@@ -3132,7 +2848,14 @@
       </a:solidFill>
       <a:round/>
     </a:ln>
-    <a:effectLst/>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+        <a:srgbClr val="000000">
+          <a:alpha val="10000"/>
+        </a:srgbClr>
+      </a:outerShdw>
+      <a:softEdge rad="12700"/>
+    </a:effectLst>
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
@@ -3272,46 +2995,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3816,7 +3499,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3843,8 +3526,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3945,509 +3628,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4834,7 +4014,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5390,23 +4570,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>170655</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>156369</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>43656</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180182</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>496092</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>161131</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>789781</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2382</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9789EEA6-6956-41BE-859F-4E0070E8A6D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{633F29B4-D8BC-4A6C-8CE0-EA2BADE99689}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5426,52 +4606,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>99218</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>84931</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1571626</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>150811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>916781</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>89694</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{633F29B4-D8BC-4A6C-8CE0-EA2BADE99689}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>87313</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>63499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>904876</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>738189</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>7938</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5492,7 +4636,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5798,10 +4942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O98"/>
+  <dimension ref="A1:Q98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5818,19 +4962,18 @@
     <col min="10" max="10" width="16.26953125" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="12" width="17.90625" customWidth="1"/>
-    <col min="14" max="14" width="22.26953125" customWidth="1"/>
-    <col min="15" max="15" width="22.6328125" customWidth="1"/>
-    <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="19" max="19" width="20.26953125" customWidth="1"/>
-    <col min="20" max="20" width="17" customWidth="1"/>
-    <col min="21" max="21" width="20.26953125" customWidth="1"/>
-    <col min="22" max="22" width="17.90625" customWidth="1"/>
-    <col min="23" max="23" width="16.54296875" customWidth="1"/>
-    <col min="25" max="25" width="21.1796875" customWidth="1"/>
-    <col min="26" max="26" width="15.7265625" customWidth="1"/>
+    <col min="14" max="15" width="22.26953125" customWidth="1"/>
+    <col min="16" max="17" width="22.6328125" customWidth="1"/>
+    <col min="20" max="20" width="20.26953125" customWidth="1"/>
+    <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="22" max="22" width="20.26953125" customWidth="1"/>
+    <col min="23" max="23" width="17.90625" customWidth="1"/>
+    <col min="24" max="24" width="16.54296875" customWidth="1"/>
+    <col min="26" max="26" width="21.1796875" customWidth="1"/>
+    <col min="27" max="27" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5843,8 +4986,14 @@
       <c r="K1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5879,8 +5028,14 @@
       <c r="O2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1011660709</v>
       </c>
@@ -5917,10 +5072,16 @@
         <v>1</v>
       </c>
       <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
         <v>235</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1011660709</v>
       </c>
@@ -5958,10 +5119,16 @@
         <v>2</v>
       </c>
       <c r="O4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1034422658</v>
       </c>
@@ -5995,10 +5162,16 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1043968983</v>
       </c>
@@ -6036,10 +5209,16 @@
         <v>5</v>
       </c>
       <c r="O6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1105019550</v>
       </c>
@@ -6076,10 +5255,16 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1176413691</v>
       </c>
@@ -6115,10 +5300,16 @@
         <v>194</v>
       </c>
       <c r="O8">
+        <v>41</v>
+      </c>
+      <c r="P8">
         <v>240</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1207339321</v>
       </c>
@@ -6156,10 +5347,16 @@
         <v>1</v>
       </c>
       <c r="O9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1237799935</v>
       </c>
@@ -6200,10 +5397,16 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1237860221</v>
       </c>
@@ -6239,10 +5442,16 @@
         <v>39</v>
       </c>
       <c r="O11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1253670590</v>
       </c>
@@ -6278,10 +5487,16 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1256766229</v>
       </c>
@@ -6317,10 +5532,16 @@
         <v>318</v>
       </c>
       <c r="O13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1266842558</v>
       </c>
@@ -6361,10 +5582,16 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1283229025</v>
       </c>
@@ -6400,10 +5627,16 @@
         <v>0</v>
       </c>
       <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1297682135</v>
       </c>
@@ -6441,10 +5674,16 @@
         <v>194</v>
       </c>
       <c r="O16">
+        <v>85</v>
+      </c>
+      <c r="P16">
         <v>6696</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q16">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1298894081</v>
       </c>
@@ -6483,10 +5722,16 @@
         <v>176</v>
       </c>
       <c r="O17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1299789239</v>
       </c>
@@ -6521,10 +5766,16 @@
         <v>19</v>
       </c>
       <c r="O18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1306259723</v>
       </c>
@@ -6542,10 +5793,16 @@
         <v>4</v>
       </c>
       <c r="O19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1314799558</v>
       </c>
@@ -6563,10 +5820,16 @@
         <v>5</v>
       </c>
       <c r="O20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1315200408</v>
       </c>
@@ -6584,10 +5847,16 @@
         <v>18</v>
       </c>
       <c r="O21">
+        <v>29</v>
+      </c>
+      <c r="P21">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1315445249</v>
       </c>
@@ -6605,10 +5874,16 @@
         <v>2</v>
       </c>
       <c r="O22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1320407798</v>
       </c>
@@ -6626,10 +5901,16 @@
         <v>4</v>
       </c>
       <c r="O23">
+        <v>3</v>
+      </c>
+      <c r="P23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1322330353</v>
       </c>
@@ -6647,10 +5928,16 @@
         <v>26</v>
       </c>
       <c r="O24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1332474676</v>
       </c>
@@ -6673,10 +5960,16 @@
         <v>5</v>
       </c>
       <c r="O25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1332980051</v>
       </c>
@@ -6694,10 +5987,16 @@
         <v>230</v>
       </c>
       <c r="O26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1333947798</v>
       </c>
@@ -6715,10 +6014,16 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1342094874</v>
       </c>
@@ -6736,10 +6041,16 @@
         <v>0</v>
       </c>
       <c r="O28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1342637455</v>
       </c>
@@ -6757,10 +6068,16 @@
         <v>0</v>
       </c>
       <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1346341630</v>
       </c>
@@ -6778,10 +6095,16 @@
         <v>8</v>
       </c>
       <c r="O30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1348000436</v>
       </c>
@@ -6799,10 +6122,16 @@
         <v>47</v>
       </c>
       <c r="O31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1351114087</v>
       </c>
@@ -6820,10 +6149,16 @@
         <v>37</v>
       </c>
       <c r="O32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1354381046</v>
       </c>
@@ -6841,10 +6176,16 @@
         <v>22</v>
       </c>
       <c r="O33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1357278519</v>
       </c>
@@ -6864,10 +6205,16 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1360718707</v>
       </c>
@@ -6885,10 +6232,16 @@
         <v>19</v>
       </c>
       <c r="O35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1370204000</v>
       </c>
@@ -6906,10 +6259,16 @@
         <v>5</v>
       </c>
       <c r="O36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1370826833</v>
       </c>
@@ -6927,10 +6286,16 @@
         <v>0</v>
       </c>
       <c r="O37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1381535033</v>
       </c>
@@ -6948,10 +6313,16 @@
         <v>42</v>
       </c>
       <c r="O38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1389397070</v>
       </c>
@@ -6971,10 +6342,16 @@
         <v>10</v>
       </c>
       <c r="O39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1390609370</v>
       </c>
@@ -6992,10 +6369,16 @@
         <v>0</v>
       </c>
       <c r="O40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1392085662</v>
       </c>
@@ -7013,10 +6396,16 @@
         <v>17</v>
       </c>
       <c r="O41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1394046157</v>
       </c>
@@ -7034,10 +6423,16 @@
         <v>55</v>
       </c>
       <c r="O42">
+        <v>9</v>
+      </c>
+      <c r="P42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1402921179</v>
       </c>
@@ -7055,10 +6450,16 @@
         <v>2</v>
       </c>
       <c r="O43">
+        <v>3</v>
+      </c>
+      <c r="P43">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1406140457</v>
       </c>
@@ -7079,10 +6480,16 @@
         <v>0</v>
       </c>
       <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1408490281</v>
       </c>
@@ -7100,10 +6507,16 @@
         <v>0</v>
       </c>
       <c r="O45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1409153544</v>
       </c>
@@ -7121,10 +6534,16 @@
         <v>1</v>
       </c>
       <c r="O46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1409750299</v>
       </c>
@@ -7142,10 +6561,16 @@
         <v>1</v>
       </c>
       <c r="O47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1413278657</v>
       </c>
@@ -7163,10 +6588,16 @@
         <v>17</v>
       </c>
       <c r="O48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1417504653</v>
       </c>
@@ -7184,10 +6615,16 @@
         <v>4</v>
       </c>
       <c r="O49">
+        <v>2</v>
+      </c>
+      <c r="P49">
         <v>129</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q49">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1417801488</v>
       </c>
@@ -7205,10 +6642,16 @@
         <v>0</v>
       </c>
       <c r="O50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1428876281</v>
       </c>
@@ -7228,10 +6671,16 @@
         <v>43</v>
       </c>
       <c r="O51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1430510164</v>
       </c>
@@ -7249,10 +6698,16 @@
         <v>0</v>
       </c>
       <c r="O52">
+        <v>4</v>
+      </c>
+      <c r="P52">
         <v>15</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q52">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1430925380</v>
       </c>
@@ -7270,10 +6725,16 @@
         <v>51</v>
       </c>
       <c r="O53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1434653100</v>
       </c>
@@ -7291,10 +6752,16 @@
         <v>9</v>
       </c>
       <c r="O54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1442661280</v>
       </c>
@@ -7312,10 +6779,16 @@
         <v>87</v>
       </c>
       <c r="O55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1449368275</v>
       </c>
@@ -7335,10 +6808,16 @@
         <v>3</v>
       </c>
       <c r="O56">
+        <v>4</v>
+      </c>
+      <c r="P56">
         <v>35</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1452698004</v>
       </c>
@@ -7360,10 +6839,16 @@
         <v>28</v>
       </c>
       <c r="O57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="Q57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1453435001</v>
       </c>
@@ -7383,10 +6868,16 @@
         <v>0</v>
       </c>
       <c r="O58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1454464594</v>
       </c>
@@ -7406,10 +6897,16 @@
         <v>0</v>
       </c>
       <c r="O59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1454782656</v>
       </c>
@@ -7427,10 +6924,16 @@
         <v>0</v>
       </c>
       <c r="O60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1457612258</v>
       </c>
@@ -7451,10 +6954,16 @@
         <v>0</v>
       </c>
       <c r="O61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1461716054</v>
       </c>
@@ -7472,10 +6981,16 @@
         <v>0</v>
       </c>
       <c r="O62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1465194671</v>
       </c>
@@ -7493,10 +7008,16 @@
         <v>16</v>
       </c>
       <c r="O63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1466016288</v>
       </c>
@@ -7514,10 +7035,16 @@
         <v>17</v>
       </c>
       <c r="O64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1467255205</v>
       </c>
@@ -7535,10 +7062,16 @@
         <v>0</v>
       </c>
       <c r="O65">
+        <v>1</v>
+      </c>
+      <c r="P65">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1477854720</v>
       </c>
@@ -7556,10 +7089,16 @@
         <v>0</v>
       </c>
       <c r="O66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1488826636</v>
       </c>
@@ -7579,10 +7118,16 @@
         <v>27</v>
       </c>
       <c r="O67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1490184268</v>
       </c>
@@ -7603,10 +7148,16 @@
         <v>1</v>
       </c>
       <c r="O68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1496071665</v>
       </c>
@@ -7624,10 +7175,16 @@
         <v>3</v>
       </c>
       <c r="O69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="P69">
+        <v>1</v>
+      </c>
+      <c r="Q69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1496349016</v>
       </c>
@@ -7645,10 +7202,16 @@
         <v>3</v>
       </c>
       <c r="O70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1498090728</v>
       </c>
@@ -7666,10 +7229,16 @@
         <v>492</v>
       </c>
       <c r="O71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1499234528</v>
       </c>
@@ -7687,10 +7256,16 @@
         <v>58</v>
       </c>
       <c r="O72">
+        <v>5</v>
+      </c>
+      <c r="P72">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q72">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1500339182</v>
       </c>
@@ -7711,10 +7286,16 @@
         <v>9</v>
       </c>
       <c r="O73">
+        <v>10</v>
+      </c>
+      <c r="P73">
         <v>66</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q73">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1500537826</v>
       </c>
@@ -7722,11 +7303,14 @@
         <v>20</v>
       </c>
       <c r="C74" s="1"/>
-      <c r="O74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="Q74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1502494929</v>
       </c>
@@ -7734,11 +7318,14 @@
         <v>1</v>
       </c>
       <c r="C75" s="1"/>
-      <c r="O75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1504609799</v>
       </c>
@@ -7746,11 +7333,14 @@
         <v>1</v>
       </c>
       <c r="C76" s="1"/>
-      <c r="O76">
+      <c r="P76">
         <v>17</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q76">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1509043599</v>
       </c>
@@ -7758,11 +7348,14 @@
         <v>1</v>
       </c>
       <c r="C77" s="1"/>
-      <c r="O77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P77">
+        <v>1</v>
+      </c>
+      <c r="Q77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1509980917</v>
       </c>
@@ -7770,11 +7363,14 @@
         <v>1</v>
       </c>
       <c r="C78" s="1"/>
-      <c r="O78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1510627730</v>
       </c>
@@ -7782,11 +7378,14 @@
         <v>1</v>
       </c>
       <c r="C79" s="1"/>
-      <c r="O79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="Q79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1513433461</v>
       </c>
@@ -7794,11 +7393,14 @@
         <v>1</v>
       </c>
       <c r="C80" s="1"/>
-      <c r="O80">
+      <c r="P80">
         <v>622</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q80">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1513502366</v>
       </c>
@@ -7806,11 +7408,14 @@
         <v>2</v>
       </c>
       <c r="C81" s="1"/>
-      <c r="O81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P81">
+        <v>0</v>
+      </c>
+      <c r="Q81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1514105016</v>
       </c>
@@ -7818,11 +7423,14 @@
         <v>1</v>
       </c>
       <c r="C82" s="1"/>
-      <c r="O82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P82">
+        <v>1</v>
+      </c>
+      <c r="Q82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1515425925</v>
       </c>
@@ -7832,11 +7440,14 @@
       <c r="C83" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O83">
+      <c r="P83">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q83">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1520258352</v>
       </c>
@@ -7844,11 +7455,14 @@
         <v>1</v>
       </c>
       <c r="C84" s="1"/>
-      <c r="O84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P84">
+        <v>0</v>
+      </c>
+      <c r="Q84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1520325457</v>
       </c>
@@ -7856,11 +7470,14 @@
         <v>1</v>
       </c>
       <c r="C85" s="1"/>
-      <c r="O85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P85">
+        <v>0</v>
+      </c>
+      <c r="Q85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>1521427474</v>
       </c>
@@ -7868,11 +7485,14 @@
         <v>4</v>
       </c>
       <c r="C86" s="1"/>
-      <c r="O86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P86">
+        <v>0</v>
+      </c>
+      <c r="Q86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>1524250714</v>
       </c>
@@ -7880,11 +7500,14 @@
         <v>1</v>
       </c>
       <c r="C87" s="1"/>
-      <c r="O87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P87">
+        <v>0</v>
+      </c>
+      <c r="Q87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1532509459</v>
       </c>
@@ -7892,11 +7515,14 @@
         <v>1</v>
       </c>
       <c r="C88" s="1"/>
-      <c r="O88">
+      <c r="P88">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1533588545</v>
       </c>
@@ -7904,11 +7530,14 @@
         <v>2</v>
       </c>
       <c r="C89" s="1"/>
-      <c r="O89">
+      <c r="P89">
         <v>103</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1540966450</v>
       </c>
@@ -7916,11 +7545,14 @@
         <v>2</v>
       </c>
       <c r="C90" s="1"/>
-      <c r="O90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P90">
+        <v>0</v>
+      </c>
+      <c r="Q90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1541901013</v>
       </c>
@@ -7928,11 +7560,14 @@
         <v>1</v>
       </c>
       <c r="C91" s="1"/>
-      <c r="O91">
+      <c r="P91">
         <v>86</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q91">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1542819512</v>
       </c>
@@ -7940,11 +7575,14 @@
         <v>1</v>
       </c>
       <c r="C92" s="1"/>
-      <c r="O92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="Q92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1543443398</v>
       </c>
@@ -7952,11 +7590,14 @@
         <v>1</v>
       </c>
       <c r="C93" s="1"/>
-      <c r="O93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P93">
+        <v>0</v>
+      </c>
+      <c r="Q93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1544565019</v>
       </c>
@@ -7964,11 +7605,14 @@
         <v>1</v>
       </c>
       <c r="C94" s="1"/>
-      <c r="O94">
+      <c r="P94">
         <v>260</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q94">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1548861450</v>
       </c>
@@ -7978,11 +7622,14 @@
       <c r="C95" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O95">
+      <c r="P95">
         <v>1920</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q95">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>1552745223</v>
       </c>
@@ -7990,11 +7637,14 @@
         <v>1</v>
       </c>
       <c r="C96" s="1"/>
-      <c r="O96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P96">
+        <v>0</v>
+      </c>
+      <c r="Q96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>1555035076</v>
       </c>
@@ -8002,11 +7652,14 @@
         <v>3</v>
       </c>
       <c r="C97" s="1"/>
-      <c r="O97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P97">
+        <v>0</v>
+      </c>
+      <c r="Q97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>1558985607</v>
       </c>
@@ -8014,8 +7667,11 @@
         <v>1</v>
       </c>
       <c r="C98" s="1"/>
-      <c r="O98">
+      <c r="P98">
         <v>17</v>
+      </c>
+      <c r="Q98">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>